<commit_message>
Fix error in pencils_9g and tulips_9g, regenerate scaffold accordingly
</commit_message>
<xml_diff>
--- a/materials/reading-ranger/stimuli/passage-error-excels/set-9b/tulips_9g.xlsx
+++ b/materials/reading-ranger/stimuli/passage-error-excels/set-9b/tulips_9g.xlsx
@@ -1120,7 +1120,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1206,8 +1206,6 @@
         <u val="none"/>
       </font>
       <numFmt numFmtId="164" formatCode="General"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
     </dxf>
     <dxf>
       <font>
@@ -1221,7 +1219,6 @@
           <bgColor rgb="FFFFCCCC"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </dxf>
     <dxf>
       <font>
@@ -1235,7 +1232,6 @@
           <bgColor rgb="FFFFFFCC"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </dxf>
   </dxfs>
   <colors>
@@ -4325,222 +4321,78 @@
       <c r="KE3" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="KF3" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KG3" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KH3" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KI3" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KJ3" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KK3" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KL3" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KM3" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KN3" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KO3" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KP3" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KQ3" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KR3" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KS3" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KT3" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KU3" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KV3" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KW3" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KX3" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KY3" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KZ3" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LA3" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LB3" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LC3" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LD3" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LE3" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LF3" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LG3" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LH3" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LI3" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LJ3" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LK3" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LL3" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LM3" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LN3" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LO3" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LP3" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LQ3" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LR3" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LS3" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LT3" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LU3" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LV3" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LW3" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LX3" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LY3" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LZ3" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MA3" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MB3" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MC3" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MD3" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="ME3" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MF3" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MG3" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MH3" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MI3" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MJ3" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MK3" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="ML3" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MM3" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MN3" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MO3" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MP3" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MQ3" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MR3" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MS3" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MT3" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MU3" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MV3" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MW3" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MX3" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MY3" s="11" t="n">
-        <v>0</v>
-      </c>
+      <c r="KF3" s="11"/>
+      <c r="KG3" s="11"/>
+      <c r="KH3" s="11"/>
+      <c r="KI3" s="11"/>
+      <c r="KJ3" s="11"/>
+      <c r="KK3" s="11"/>
+      <c r="KL3" s="11"/>
+      <c r="KM3" s="11"/>
+      <c r="KN3" s="11"/>
+      <c r="KO3" s="11"/>
+      <c r="KP3" s="11"/>
+      <c r="KQ3" s="11"/>
+      <c r="KR3" s="11"/>
+      <c r="KS3" s="11"/>
+      <c r="KT3" s="11"/>
+      <c r="KU3" s="11"/>
+      <c r="KV3" s="11"/>
+      <c r="KW3" s="11"/>
+      <c r="KX3" s="11"/>
+      <c r="KY3" s="11"/>
+      <c r="KZ3" s="11"/>
+      <c r="LA3" s="11"/>
+      <c r="LB3" s="11"/>
+      <c r="LC3" s="11"/>
+      <c r="LD3" s="11"/>
+      <c r="LE3" s="11"/>
+      <c r="LF3" s="11"/>
+      <c r="LG3" s="11"/>
+      <c r="LH3" s="11"/>
+      <c r="LI3" s="11"/>
+      <c r="LJ3" s="11"/>
+      <c r="LK3" s="11"/>
+      <c r="LL3" s="11"/>
+      <c r="LM3" s="11"/>
+      <c r="LN3" s="11"/>
+      <c r="LO3" s="11"/>
+      <c r="LP3" s="11"/>
+      <c r="LQ3" s="11"/>
+      <c r="LR3" s="11"/>
+      <c r="LS3" s="11"/>
+      <c r="LT3" s="11"/>
+      <c r="LU3" s="11"/>
+      <c r="LV3" s="11"/>
+      <c r="LW3" s="11"/>
+      <c r="LX3" s="11"/>
+      <c r="LY3" s="11"/>
+      <c r="LZ3" s="11"/>
+      <c r="MA3" s="11"/>
+      <c r="MB3" s="11"/>
+      <c r="MC3" s="11"/>
+      <c r="MD3" s="11"/>
+      <c r="ME3" s="11"/>
+      <c r="MF3" s="11"/>
+      <c r="MG3" s="11"/>
+      <c r="MH3" s="11"/>
+      <c r="MI3" s="11"/>
+      <c r="MJ3" s="11"/>
+      <c r="MK3" s="11"/>
+      <c r="ML3" s="11"/>
+      <c r="MM3" s="11"/>
+      <c r="MN3" s="11"/>
+      <c r="MO3" s="11"/>
+      <c r="MP3" s="11"/>
+      <c r="MQ3" s="11"/>
+      <c r="MR3" s="11"/>
+      <c r="MS3" s="11"/>
+      <c r="MT3" s="11"/>
+      <c r="MU3" s="11"/>
+      <c r="MV3" s="11"/>
+      <c r="MW3" s="11"/>
+      <c r="MX3" s="11"/>
+      <c r="MY3" s="11"/>
       <c r="MZ3" s="13"/>
       <c r="NA3" s="13"/>
       <c r="NB3" s="13"/>
@@ -5424,222 +5276,78 @@
       <c r="KE4" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="KF4" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KG4" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KH4" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KI4" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KJ4" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KK4" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KL4" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KM4" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KN4" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KO4" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KP4" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KQ4" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KR4" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KS4" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KT4" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KU4" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KV4" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KW4" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KX4" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KY4" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KZ4" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LA4" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LB4" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LC4" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LD4" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LE4" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LF4" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LG4" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LH4" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LI4" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LJ4" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LK4" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LL4" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LM4" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LN4" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LO4" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LP4" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LQ4" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LR4" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LS4" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LT4" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LU4" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LV4" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LW4" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LX4" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LY4" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LZ4" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MA4" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MB4" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MC4" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MD4" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="ME4" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MF4" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MG4" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MH4" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MI4" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MJ4" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MK4" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="ML4" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MM4" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MN4" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MO4" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MP4" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MQ4" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MR4" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MS4" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MT4" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MU4" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MV4" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MW4" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MX4" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MY4" s="11" t="n">
-        <v>0</v>
-      </c>
+      <c r="KF4" s="11"/>
+      <c r="KG4" s="11"/>
+      <c r="KH4" s="11"/>
+      <c r="KI4" s="11"/>
+      <c r="KJ4" s="11"/>
+      <c r="KK4" s="11"/>
+      <c r="KL4" s="11"/>
+      <c r="KM4" s="11"/>
+      <c r="KN4" s="11"/>
+      <c r="KO4" s="11"/>
+      <c r="KP4" s="11"/>
+      <c r="KQ4" s="11"/>
+      <c r="KR4" s="11"/>
+      <c r="KS4" s="11"/>
+      <c r="KT4" s="11"/>
+      <c r="KU4" s="11"/>
+      <c r="KV4" s="11"/>
+      <c r="KW4" s="11"/>
+      <c r="KX4" s="11"/>
+      <c r="KY4" s="11"/>
+      <c r="KZ4" s="11"/>
+      <c r="LA4" s="11"/>
+      <c r="LB4" s="11"/>
+      <c r="LC4" s="11"/>
+      <c r="LD4" s="11"/>
+      <c r="LE4" s="11"/>
+      <c r="LF4" s="11"/>
+      <c r="LG4" s="11"/>
+      <c r="LH4" s="11"/>
+      <c r="LI4" s="11"/>
+      <c r="LJ4" s="11"/>
+      <c r="LK4" s="11"/>
+      <c r="LL4" s="11"/>
+      <c r="LM4" s="11"/>
+      <c r="LN4" s="11"/>
+      <c r="LO4" s="11"/>
+      <c r="LP4" s="11"/>
+      <c r="LQ4" s="11"/>
+      <c r="LR4" s="11"/>
+      <c r="LS4" s="11"/>
+      <c r="LT4" s="11"/>
+      <c r="LU4" s="11"/>
+      <c r="LV4" s="11"/>
+      <c r="LW4" s="11"/>
+      <c r="LX4" s="11"/>
+      <c r="LY4" s="11"/>
+      <c r="LZ4" s="11"/>
+      <c r="MA4" s="11"/>
+      <c r="MB4" s="11"/>
+      <c r="MC4" s="11"/>
+      <c r="MD4" s="11"/>
+      <c r="ME4" s="11"/>
+      <c r="MF4" s="11"/>
+      <c r="MG4" s="11"/>
+      <c r="MH4" s="11"/>
+      <c r="MI4" s="11"/>
+      <c r="MJ4" s="11"/>
+      <c r="MK4" s="11"/>
+      <c r="ML4" s="11"/>
+      <c r="MM4" s="11"/>
+      <c r="MN4" s="11"/>
+      <c r="MO4" s="11"/>
+      <c r="MP4" s="11"/>
+      <c r="MQ4" s="11"/>
+      <c r="MR4" s="11"/>
+      <c r="MS4" s="11"/>
+      <c r="MT4" s="11"/>
+      <c r="MU4" s="11"/>
+      <c r="MV4" s="11"/>
+      <c r="MW4" s="11"/>
+      <c r="MX4" s="11"/>
+      <c r="MY4" s="11"/>
       <c r="MZ4" s="13"/>
       <c r="NA4" s="13"/>
       <c r="NB4" s="13"/>
@@ -6523,222 +6231,78 @@
       <c r="KE5" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="KF5" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KG5" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KH5" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KI5" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KJ5" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KK5" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KL5" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KM5" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KN5" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KO5" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KP5" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KQ5" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KR5" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KS5" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KT5" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KU5" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KV5" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KW5" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KX5" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KY5" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KZ5" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LA5" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LB5" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LC5" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LD5" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LE5" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LF5" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LG5" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LH5" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LI5" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LJ5" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LK5" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LL5" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LM5" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LN5" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LO5" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LP5" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LQ5" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LR5" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LS5" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LT5" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LU5" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LV5" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LW5" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LX5" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LY5" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LZ5" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MA5" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MB5" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MC5" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MD5" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="ME5" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MF5" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MG5" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MH5" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MI5" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MJ5" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MK5" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="ML5" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MM5" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MN5" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MO5" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MP5" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MQ5" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MR5" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MS5" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MT5" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MU5" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MV5" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MW5" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MX5" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MY5" s="11" t="n">
-        <v>0</v>
-      </c>
+      <c r="KF5" s="11"/>
+      <c r="KG5" s="11"/>
+      <c r="KH5" s="11"/>
+      <c r="KI5" s="11"/>
+      <c r="KJ5" s="11"/>
+      <c r="KK5" s="11"/>
+      <c r="KL5" s="11"/>
+      <c r="KM5" s="11"/>
+      <c r="KN5" s="11"/>
+      <c r="KO5" s="11"/>
+      <c r="KP5" s="11"/>
+      <c r="KQ5" s="11"/>
+      <c r="KR5" s="11"/>
+      <c r="KS5" s="11"/>
+      <c r="KT5" s="11"/>
+      <c r="KU5" s="11"/>
+      <c r="KV5" s="11"/>
+      <c r="KW5" s="11"/>
+      <c r="KX5" s="11"/>
+      <c r="KY5" s="11"/>
+      <c r="KZ5" s="11"/>
+      <c r="LA5" s="11"/>
+      <c r="LB5" s="11"/>
+      <c r="LC5" s="11"/>
+      <c r="LD5" s="11"/>
+      <c r="LE5" s="11"/>
+      <c r="LF5" s="11"/>
+      <c r="LG5" s="11"/>
+      <c r="LH5" s="11"/>
+      <c r="LI5" s="11"/>
+      <c r="LJ5" s="11"/>
+      <c r="LK5" s="11"/>
+      <c r="LL5" s="11"/>
+      <c r="LM5" s="11"/>
+      <c r="LN5" s="11"/>
+      <c r="LO5" s="11"/>
+      <c r="LP5" s="11"/>
+      <c r="LQ5" s="11"/>
+      <c r="LR5" s="11"/>
+      <c r="LS5" s="11"/>
+      <c r="LT5" s="11"/>
+      <c r="LU5" s="11"/>
+      <c r="LV5" s="11"/>
+      <c r="LW5" s="11"/>
+      <c r="LX5" s="11"/>
+      <c r="LY5" s="11"/>
+      <c r="LZ5" s="11"/>
+      <c r="MA5" s="11"/>
+      <c r="MB5" s="11"/>
+      <c r="MC5" s="11"/>
+      <c r="MD5" s="11"/>
+      <c r="ME5" s="11"/>
+      <c r="MF5" s="11"/>
+      <c r="MG5" s="11"/>
+      <c r="MH5" s="11"/>
+      <c r="MI5" s="11"/>
+      <c r="MJ5" s="11"/>
+      <c r="MK5" s="11"/>
+      <c r="ML5" s="11"/>
+      <c r="MM5" s="11"/>
+      <c r="MN5" s="11"/>
+      <c r="MO5" s="11"/>
+      <c r="MP5" s="11"/>
+      <c r="MQ5" s="11"/>
+      <c r="MR5" s="11"/>
+      <c r="MS5" s="11"/>
+      <c r="MT5" s="11"/>
+      <c r="MU5" s="11"/>
+      <c r="MV5" s="11"/>
+      <c r="MW5" s="11"/>
+      <c r="MX5" s="11"/>
+      <c r="MY5" s="11"/>
       <c r="MZ5" s="13"/>
       <c r="NA5" s="13"/>
       <c r="NB5" s="13"/>
@@ -7622,222 +7186,78 @@
       <c r="KE6" s="16" t="n">
         <v>0</v>
       </c>
-      <c r="KF6" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="KG6" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="KH6" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="KI6" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="KJ6" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="KK6" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="KL6" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="KM6" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="KN6" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="KO6" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="KP6" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="KQ6" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="KR6" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="KS6" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="KT6" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="KU6" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="KV6" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="KW6" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="KX6" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="KY6" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="KZ6" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="LA6" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="LB6" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="LC6" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="LD6" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="LE6" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="LF6" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="LG6" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="LH6" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="LI6" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="LJ6" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="LK6" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="LL6" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="LM6" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="LN6" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="LO6" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="LP6" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="LQ6" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="LR6" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="LS6" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="LT6" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="LU6" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="LV6" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="LW6" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="LX6" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="LY6" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="LZ6" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="MA6" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="MB6" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="MC6" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="MD6" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="ME6" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="MF6" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="MG6" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="MH6" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="MI6" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="MJ6" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="MK6" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="ML6" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="MM6" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="MN6" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="MO6" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="MP6" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="MQ6" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="MR6" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="MS6" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="MT6" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="MU6" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="MV6" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="MW6" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="MX6" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="MY6" s="16" t="n">
-        <v>0</v>
-      </c>
+      <c r="KF6" s="16"/>
+      <c r="KG6" s="16"/>
+      <c r="KH6" s="16"/>
+      <c r="KI6" s="16"/>
+      <c r="KJ6" s="16"/>
+      <c r="KK6" s="16"/>
+      <c r="KL6" s="16"/>
+      <c r="KM6" s="16"/>
+      <c r="KN6" s="16"/>
+      <c r="KO6" s="16"/>
+      <c r="KP6" s="16"/>
+      <c r="KQ6" s="16"/>
+      <c r="KR6" s="16"/>
+      <c r="KS6" s="16"/>
+      <c r="KT6" s="16"/>
+      <c r="KU6" s="16"/>
+      <c r="KV6" s="16"/>
+      <c r="KW6" s="16"/>
+      <c r="KX6" s="16"/>
+      <c r="KY6" s="16"/>
+      <c r="KZ6" s="16"/>
+      <c r="LA6" s="16"/>
+      <c r="LB6" s="16"/>
+      <c r="LC6" s="16"/>
+      <c r="LD6" s="16"/>
+      <c r="LE6" s="16"/>
+      <c r="LF6" s="16"/>
+      <c r="LG6" s="16"/>
+      <c r="LH6" s="16"/>
+      <c r="LI6" s="16"/>
+      <c r="LJ6" s="16"/>
+      <c r="LK6" s="16"/>
+      <c r="LL6" s="16"/>
+      <c r="LM6" s="16"/>
+      <c r="LN6" s="16"/>
+      <c r="LO6" s="16"/>
+      <c r="LP6" s="16"/>
+      <c r="LQ6" s="16"/>
+      <c r="LR6" s="16"/>
+      <c r="LS6" s="16"/>
+      <c r="LT6" s="16"/>
+      <c r="LU6" s="16"/>
+      <c r="LV6" s="16"/>
+      <c r="LW6" s="16"/>
+      <c r="LX6" s="16"/>
+      <c r="LY6" s="16"/>
+      <c r="LZ6" s="16"/>
+      <c r="MA6" s="16"/>
+      <c r="MB6" s="16"/>
+      <c r="MC6" s="16"/>
+      <c r="MD6" s="16"/>
+      <c r="ME6" s="16"/>
+      <c r="MF6" s="16"/>
+      <c r="MG6" s="16"/>
+      <c r="MH6" s="16"/>
+      <c r="MI6" s="16"/>
+      <c r="MJ6" s="16"/>
+      <c r="MK6" s="16"/>
+      <c r="ML6" s="16"/>
+      <c r="MM6" s="16"/>
+      <c r="MN6" s="16"/>
+      <c r="MO6" s="16"/>
+      <c r="MP6" s="16"/>
+      <c r="MQ6" s="16"/>
+      <c r="MR6" s="16"/>
+      <c r="MS6" s="16"/>
+      <c r="MT6" s="16"/>
+      <c r="MU6" s="16"/>
+      <c r="MV6" s="16"/>
+      <c r="MW6" s="16"/>
+      <c r="MX6" s="16"/>
+      <c r="MY6" s="16"/>
       <c r="MZ6" s="18"/>
       <c r="NA6" s="18"/>
       <c r="NB6" s="18"/>
@@ -8721,222 +8141,78 @@
       <c r="KE7" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="KF7" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KG7" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KH7" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KI7" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KJ7" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KK7" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KL7" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KM7" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KN7" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KO7" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KP7" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KQ7" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KR7" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KS7" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KT7" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KU7" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KV7" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KW7" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KX7" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KY7" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KZ7" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LA7" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LB7" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LC7" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LD7" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LE7" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LF7" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LG7" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LH7" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LI7" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LJ7" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LK7" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LL7" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LM7" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LN7" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LO7" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LP7" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LQ7" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LR7" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LS7" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LT7" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LU7" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LV7" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LW7" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LX7" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LY7" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LZ7" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MA7" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MB7" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MC7" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MD7" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="ME7" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MF7" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MG7" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MH7" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MI7" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MJ7" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MK7" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="ML7" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MM7" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MN7" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MO7" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MP7" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MQ7" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MR7" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MS7" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MT7" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MU7" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MV7" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MW7" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MX7" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MY7" s="11" t="n">
-        <v>0</v>
-      </c>
+      <c r="KF7" s="11"/>
+      <c r="KG7" s="11"/>
+      <c r="KH7" s="11"/>
+      <c r="KI7" s="11"/>
+      <c r="KJ7" s="11"/>
+      <c r="KK7" s="11"/>
+      <c r="KL7" s="11"/>
+      <c r="KM7" s="11"/>
+      <c r="KN7" s="11"/>
+      <c r="KO7" s="11"/>
+      <c r="KP7" s="11"/>
+      <c r="KQ7" s="11"/>
+      <c r="KR7" s="11"/>
+      <c r="KS7" s="11"/>
+      <c r="KT7" s="11"/>
+      <c r="KU7" s="11"/>
+      <c r="KV7" s="11"/>
+      <c r="KW7" s="11"/>
+      <c r="KX7" s="11"/>
+      <c r="KY7" s="11"/>
+      <c r="KZ7" s="11"/>
+      <c r="LA7" s="11"/>
+      <c r="LB7" s="11"/>
+      <c r="LC7" s="11"/>
+      <c r="LD7" s="11"/>
+      <c r="LE7" s="11"/>
+      <c r="LF7" s="11"/>
+      <c r="LG7" s="11"/>
+      <c r="LH7" s="11"/>
+      <c r="LI7" s="11"/>
+      <c r="LJ7" s="11"/>
+      <c r="LK7" s="11"/>
+      <c r="LL7" s="11"/>
+      <c r="LM7" s="11"/>
+      <c r="LN7" s="11"/>
+      <c r="LO7" s="11"/>
+      <c r="LP7" s="11"/>
+      <c r="LQ7" s="11"/>
+      <c r="LR7" s="11"/>
+      <c r="LS7" s="11"/>
+      <c r="LT7" s="11"/>
+      <c r="LU7" s="11"/>
+      <c r="LV7" s="11"/>
+      <c r="LW7" s="11"/>
+      <c r="LX7" s="11"/>
+      <c r="LY7" s="11"/>
+      <c r="LZ7" s="11"/>
+      <c r="MA7" s="11"/>
+      <c r="MB7" s="11"/>
+      <c r="MC7" s="11"/>
+      <c r="MD7" s="11"/>
+      <c r="ME7" s="11"/>
+      <c r="MF7" s="11"/>
+      <c r="MG7" s="11"/>
+      <c r="MH7" s="11"/>
+      <c r="MI7" s="11"/>
+      <c r="MJ7" s="11"/>
+      <c r="MK7" s="11"/>
+      <c r="ML7" s="11"/>
+      <c r="MM7" s="11"/>
+      <c r="MN7" s="11"/>
+      <c r="MO7" s="11"/>
+      <c r="MP7" s="11"/>
+      <c r="MQ7" s="11"/>
+      <c r="MR7" s="11"/>
+      <c r="MS7" s="11"/>
+      <c r="MT7" s="11"/>
+      <c r="MU7" s="11"/>
+      <c r="MV7" s="11"/>
+      <c r="MW7" s="11"/>
+      <c r="MX7" s="11"/>
+      <c r="MY7" s="11"/>
       <c r="MZ7" s="13"/>
       <c r="NA7" s="13"/>
       <c r="NB7" s="13"/>
@@ -9820,222 +9096,78 @@
       <c r="KE8" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="KF8" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KG8" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KH8" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KI8" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KJ8" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KK8" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KL8" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KM8" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KN8" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KO8" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KP8" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KQ8" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KR8" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KS8" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KT8" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KU8" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KV8" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KW8" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KX8" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KY8" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KZ8" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LA8" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LB8" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LC8" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LD8" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LE8" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LF8" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LG8" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LH8" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LI8" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LJ8" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LK8" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LL8" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LM8" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LN8" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LO8" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LP8" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LQ8" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LR8" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LS8" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LT8" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LU8" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LV8" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LW8" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LX8" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LY8" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LZ8" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MA8" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MB8" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MC8" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MD8" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="ME8" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MF8" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MG8" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MH8" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MI8" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MJ8" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MK8" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="ML8" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MM8" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MN8" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MO8" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MP8" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MQ8" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MR8" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MS8" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MT8" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MU8" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MV8" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MW8" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MX8" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MY8" s="11" t="n">
-        <v>0</v>
-      </c>
+      <c r="KF8" s="11"/>
+      <c r="KG8" s="11"/>
+      <c r="KH8" s="11"/>
+      <c r="KI8" s="11"/>
+      <c r="KJ8" s="11"/>
+      <c r="KK8" s="11"/>
+      <c r="KL8" s="11"/>
+      <c r="KM8" s="11"/>
+      <c r="KN8" s="11"/>
+      <c r="KO8" s="11"/>
+      <c r="KP8" s="11"/>
+      <c r="KQ8" s="11"/>
+      <c r="KR8" s="11"/>
+      <c r="KS8" s="11"/>
+      <c r="KT8" s="11"/>
+      <c r="KU8" s="11"/>
+      <c r="KV8" s="11"/>
+      <c r="KW8" s="11"/>
+      <c r="KX8" s="11"/>
+      <c r="KY8" s="11"/>
+      <c r="KZ8" s="11"/>
+      <c r="LA8" s="11"/>
+      <c r="LB8" s="11"/>
+      <c r="LC8" s="11"/>
+      <c r="LD8" s="11"/>
+      <c r="LE8" s="11"/>
+      <c r="LF8" s="11"/>
+      <c r="LG8" s="11"/>
+      <c r="LH8" s="11"/>
+      <c r="LI8" s="11"/>
+      <c r="LJ8" s="11"/>
+      <c r="LK8" s="11"/>
+      <c r="LL8" s="11"/>
+      <c r="LM8" s="11"/>
+      <c r="LN8" s="11"/>
+      <c r="LO8" s="11"/>
+      <c r="LP8" s="11"/>
+      <c r="LQ8" s="11"/>
+      <c r="LR8" s="11"/>
+      <c r="LS8" s="11"/>
+      <c r="LT8" s="11"/>
+      <c r="LU8" s="11"/>
+      <c r="LV8" s="11"/>
+      <c r="LW8" s="11"/>
+      <c r="LX8" s="11"/>
+      <c r="LY8" s="11"/>
+      <c r="LZ8" s="11"/>
+      <c r="MA8" s="11"/>
+      <c r="MB8" s="11"/>
+      <c r="MC8" s="11"/>
+      <c r="MD8" s="11"/>
+      <c r="ME8" s="11"/>
+      <c r="MF8" s="11"/>
+      <c r="MG8" s="11"/>
+      <c r="MH8" s="11"/>
+      <c r="MI8" s="11"/>
+      <c r="MJ8" s="11"/>
+      <c r="MK8" s="11"/>
+      <c r="ML8" s="11"/>
+      <c r="MM8" s="11"/>
+      <c r="MN8" s="11"/>
+      <c r="MO8" s="11"/>
+      <c r="MP8" s="11"/>
+      <c r="MQ8" s="11"/>
+      <c r="MR8" s="11"/>
+      <c r="MS8" s="11"/>
+      <c r="MT8" s="11"/>
+      <c r="MU8" s="11"/>
+      <c r="MV8" s="11"/>
+      <c r="MW8" s="11"/>
+      <c r="MX8" s="11"/>
+      <c r="MY8" s="11"/>
       <c r="MZ8" s="13"/>
       <c r="NA8" s="13"/>
       <c r="NB8" s="13"/>
@@ -10919,222 +10051,78 @@
       <c r="KE9" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="KF9" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KG9" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KH9" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KI9" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KJ9" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KK9" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KL9" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KM9" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KN9" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KO9" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KP9" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KQ9" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KR9" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KS9" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KT9" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KU9" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KV9" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KW9" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KX9" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KY9" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KZ9" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LA9" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LB9" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LC9" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LD9" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LE9" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LF9" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LG9" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LH9" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LI9" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LJ9" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LK9" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LL9" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LM9" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LN9" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LO9" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LP9" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LQ9" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LR9" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LS9" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LT9" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LU9" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LV9" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LW9" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LX9" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LY9" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LZ9" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MA9" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MB9" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MC9" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MD9" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="ME9" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MF9" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MG9" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MH9" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MI9" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MJ9" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MK9" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="ML9" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MM9" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MN9" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MO9" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MP9" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MQ9" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MR9" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MS9" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MT9" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MU9" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MV9" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MW9" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MX9" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MY9" s="11" t="n">
-        <v>0</v>
-      </c>
+      <c r="KF9" s="11"/>
+      <c r="KG9" s="11"/>
+      <c r="KH9" s="11"/>
+      <c r="KI9" s="11"/>
+      <c r="KJ9" s="11"/>
+      <c r="KK9" s="11"/>
+      <c r="KL9" s="11"/>
+      <c r="KM9" s="11"/>
+      <c r="KN9" s="11"/>
+      <c r="KO9" s="11"/>
+      <c r="KP9" s="11"/>
+      <c r="KQ9" s="11"/>
+      <c r="KR9" s="11"/>
+      <c r="KS9" s="11"/>
+      <c r="KT9" s="11"/>
+      <c r="KU9" s="11"/>
+      <c r="KV9" s="11"/>
+      <c r="KW9" s="11"/>
+      <c r="KX9" s="11"/>
+      <c r="KY9" s="11"/>
+      <c r="KZ9" s="11"/>
+      <c r="LA9" s="11"/>
+      <c r="LB9" s="11"/>
+      <c r="LC9" s="11"/>
+      <c r="LD9" s="11"/>
+      <c r="LE9" s="11"/>
+      <c r="LF9" s="11"/>
+      <c r="LG9" s="11"/>
+      <c r="LH9" s="11"/>
+      <c r="LI9" s="11"/>
+      <c r="LJ9" s="11"/>
+      <c r="LK9" s="11"/>
+      <c r="LL9" s="11"/>
+      <c r="LM9" s="11"/>
+      <c r="LN9" s="11"/>
+      <c r="LO9" s="11"/>
+      <c r="LP9" s="11"/>
+      <c r="LQ9" s="11"/>
+      <c r="LR9" s="11"/>
+      <c r="LS9" s="11"/>
+      <c r="LT9" s="11"/>
+      <c r="LU9" s="11"/>
+      <c r="LV9" s="11"/>
+      <c r="LW9" s="11"/>
+      <c r="LX9" s="11"/>
+      <c r="LY9" s="11"/>
+      <c r="LZ9" s="11"/>
+      <c r="MA9" s="11"/>
+      <c r="MB9" s="11"/>
+      <c r="MC9" s="11"/>
+      <c r="MD9" s="11"/>
+      <c r="ME9" s="11"/>
+      <c r="MF9" s="11"/>
+      <c r="MG9" s="11"/>
+      <c r="MH9" s="11"/>
+      <c r="MI9" s="11"/>
+      <c r="MJ9" s="11"/>
+      <c r="MK9" s="11"/>
+      <c r="ML9" s="11"/>
+      <c r="MM9" s="11"/>
+      <c r="MN9" s="11"/>
+      <c r="MO9" s="11"/>
+      <c r="MP9" s="11"/>
+      <c r="MQ9" s="11"/>
+      <c r="MR9" s="11"/>
+      <c r="MS9" s="11"/>
+      <c r="MT9" s="11"/>
+      <c r="MU9" s="11"/>
+      <c r="MV9" s="11"/>
+      <c r="MW9" s="11"/>
+      <c r="MX9" s="11"/>
+      <c r="MY9" s="11"/>
       <c r="MZ9" s="13"/>
       <c r="NA9" s="13"/>
       <c r="NB9" s="13"/>
@@ -12018,222 +11006,78 @@
       <c r="KE10" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="KF10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KG10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KH10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KI10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KJ10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KK10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KL10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KM10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KN10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KO10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KP10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KQ10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KR10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KS10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KT10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KU10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KV10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KW10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KX10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KY10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KZ10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LA10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LB10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LC10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LD10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LE10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LF10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LG10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LH10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LI10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LJ10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LK10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LL10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LM10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LN10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LO10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LP10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LQ10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LR10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LS10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LT10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LU10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LV10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LW10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LX10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LY10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LZ10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MA10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MB10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MC10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MD10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="ME10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MF10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MG10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MH10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MI10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MJ10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MK10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="ML10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MM10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MN10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MO10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MP10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MQ10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MR10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MS10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MT10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MU10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MV10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MW10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MX10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MY10" s="11" t="n">
-        <v>0</v>
-      </c>
+      <c r="KF10" s="11"/>
+      <c r="KG10" s="11"/>
+      <c r="KH10" s="11"/>
+      <c r="KI10" s="11"/>
+      <c r="KJ10" s="11"/>
+      <c r="KK10" s="11"/>
+      <c r="KL10" s="11"/>
+      <c r="KM10" s="11"/>
+      <c r="KN10" s="11"/>
+      <c r="KO10" s="11"/>
+      <c r="KP10" s="11"/>
+      <c r="KQ10" s="11"/>
+      <c r="KR10" s="11"/>
+      <c r="KS10" s="11"/>
+      <c r="KT10" s="11"/>
+      <c r="KU10" s="11"/>
+      <c r="KV10" s="11"/>
+      <c r="KW10" s="11"/>
+      <c r="KX10" s="11"/>
+      <c r="KY10" s="11"/>
+      <c r="KZ10" s="11"/>
+      <c r="LA10" s="11"/>
+      <c r="LB10" s="11"/>
+      <c r="LC10" s="11"/>
+      <c r="LD10" s="11"/>
+      <c r="LE10" s="11"/>
+      <c r="LF10" s="11"/>
+      <c r="LG10" s="11"/>
+      <c r="LH10" s="11"/>
+      <c r="LI10" s="11"/>
+      <c r="LJ10" s="11"/>
+      <c r="LK10" s="11"/>
+      <c r="LL10" s="11"/>
+      <c r="LM10" s="11"/>
+      <c r="LN10" s="11"/>
+      <c r="LO10" s="11"/>
+      <c r="LP10" s="11"/>
+      <c r="LQ10" s="11"/>
+      <c r="LR10" s="11"/>
+      <c r="LS10" s="11"/>
+      <c r="LT10" s="11"/>
+      <c r="LU10" s="11"/>
+      <c r="LV10" s="11"/>
+      <c r="LW10" s="11"/>
+      <c r="LX10" s="11"/>
+      <c r="LY10" s="11"/>
+      <c r="LZ10" s="11"/>
+      <c r="MA10" s="11"/>
+      <c r="MB10" s="11"/>
+      <c r="MC10" s="11"/>
+      <c r="MD10" s="11"/>
+      <c r="ME10" s="11"/>
+      <c r="MF10" s="11"/>
+      <c r="MG10" s="11"/>
+      <c r="MH10" s="11"/>
+      <c r="MI10" s="11"/>
+      <c r="MJ10" s="11"/>
+      <c r="MK10" s="11"/>
+      <c r="ML10" s="11"/>
+      <c r="MM10" s="11"/>
+      <c r="MN10" s="11"/>
+      <c r="MO10" s="11"/>
+      <c r="MP10" s="11"/>
+      <c r="MQ10" s="11"/>
+      <c r="MR10" s="11"/>
+      <c r="MS10" s="11"/>
+      <c r="MT10" s="11"/>
+      <c r="MU10" s="11"/>
+      <c r="MV10" s="11"/>
+      <c r="MW10" s="11"/>
+      <c r="MX10" s="11"/>
+      <c r="MY10" s="11"/>
       <c r="MZ10" s="13"/>
       <c r="NA10" s="13"/>
       <c r="NB10" s="13"/>
@@ -13117,222 +11961,78 @@
       <c r="KE11" s="21" t="n">
         <v>0</v>
       </c>
-      <c r="KF11" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="KG11" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="KH11" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="KI11" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="KJ11" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="KK11" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="KL11" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="KM11" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="KN11" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="KO11" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="KP11" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="KQ11" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="KR11" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="KS11" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="KT11" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="KU11" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="KV11" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="KW11" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="KX11" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="KY11" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="KZ11" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="LA11" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="LB11" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="LC11" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="LD11" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="LE11" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="LF11" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="LG11" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="LH11" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="LI11" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="LJ11" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="LK11" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="LL11" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="LM11" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="LN11" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="LO11" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="LP11" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="LQ11" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="LR11" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="LS11" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="LT11" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="LU11" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="LV11" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="LW11" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="LX11" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="LY11" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="LZ11" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="MA11" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="MB11" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="MC11" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="MD11" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="ME11" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="MF11" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="MG11" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="MH11" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="MI11" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="MJ11" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="MK11" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="ML11" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="MM11" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="MN11" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="MO11" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="MP11" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="MQ11" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="MR11" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="MS11" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="MT11" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="MU11" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="MV11" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="MW11" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="MX11" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="MY11" s="21" t="n">
-        <v>0</v>
-      </c>
+      <c r="KF11" s="21"/>
+      <c r="KG11" s="21"/>
+      <c r="KH11" s="21"/>
+      <c r="KI11" s="21"/>
+      <c r="KJ11" s="21"/>
+      <c r="KK11" s="21"/>
+      <c r="KL11" s="21"/>
+      <c r="KM11" s="21"/>
+      <c r="KN11" s="21"/>
+      <c r="KO11" s="21"/>
+      <c r="KP11" s="21"/>
+      <c r="KQ11" s="21"/>
+      <c r="KR11" s="21"/>
+      <c r="KS11" s="21"/>
+      <c r="KT11" s="21"/>
+      <c r="KU11" s="21"/>
+      <c r="KV11" s="21"/>
+      <c r="KW11" s="21"/>
+      <c r="KX11" s="21"/>
+      <c r="KY11" s="21"/>
+      <c r="KZ11" s="21"/>
+      <c r="LA11" s="21"/>
+      <c r="LB11" s="21"/>
+      <c r="LC11" s="21"/>
+      <c r="LD11" s="21"/>
+      <c r="LE11" s="21"/>
+      <c r="LF11" s="21"/>
+      <c r="LG11" s="21"/>
+      <c r="LH11" s="21"/>
+      <c r="LI11" s="21"/>
+      <c r="LJ11" s="21"/>
+      <c r="LK11" s="21"/>
+      <c r="LL11" s="21"/>
+      <c r="LM11" s="21"/>
+      <c r="LN11" s="21"/>
+      <c r="LO11" s="21"/>
+      <c r="LP11" s="21"/>
+      <c r="LQ11" s="21"/>
+      <c r="LR11" s="21"/>
+      <c r="LS11" s="21"/>
+      <c r="LT11" s="21"/>
+      <c r="LU11" s="21"/>
+      <c r="LV11" s="21"/>
+      <c r="LW11" s="21"/>
+      <c r="LX11" s="21"/>
+      <c r="LY11" s="21"/>
+      <c r="LZ11" s="21"/>
+      <c r="MA11" s="21"/>
+      <c r="MB11" s="21"/>
+      <c r="MC11" s="21"/>
+      <c r="MD11" s="21"/>
+      <c r="ME11" s="21"/>
+      <c r="MF11" s="21"/>
+      <c r="MG11" s="21"/>
+      <c r="MH11" s="21"/>
+      <c r="MI11" s="21"/>
+      <c r="MJ11" s="21"/>
+      <c r="MK11" s="21"/>
+      <c r="ML11" s="21"/>
+      <c r="MM11" s="21"/>
+      <c r="MN11" s="21"/>
+      <c r="MO11" s="21"/>
+      <c r="MP11" s="21"/>
+      <c r="MQ11" s="21"/>
+      <c r="MR11" s="21"/>
+      <c r="MS11" s="21"/>
+      <c r="MT11" s="21"/>
+      <c r="MU11" s="21"/>
+      <c r="MV11" s="21"/>
+      <c r="MW11" s="21"/>
+      <c r="MX11" s="21"/>
+      <c r="MY11" s="21"/>
       <c r="MZ11" s="23"/>
       <c r="NA11" s="23"/>
       <c r="NB11" s="23"/>
@@ -14216,222 +12916,78 @@
       <c r="KE12" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="KF12" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KG12" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KH12" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KI12" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KJ12" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KK12" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KL12" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KM12" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KN12" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KO12" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KP12" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KQ12" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KR12" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KS12" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KT12" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KU12" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KV12" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KW12" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KX12" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KY12" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KZ12" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LA12" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LB12" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LC12" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LD12" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LE12" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LF12" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LG12" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LH12" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LI12" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LJ12" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LK12" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LL12" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LM12" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LN12" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LO12" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LP12" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LQ12" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LR12" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LS12" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LT12" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LU12" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LV12" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LW12" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LX12" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LY12" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LZ12" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MA12" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MB12" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MC12" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MD12" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="ME12" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MF12" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MG12" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MH12" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MI12" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MJ12" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MK12" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="ML12" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MM12" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MN12" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MO12" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MP12" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MQ12" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MR12" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MS12" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MT12" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MU12" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MV12" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MW12" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MX12" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MY12" s="11" t="n">
-        <v>0</v>
-      </c>
+      <c r="KF12" s="11"/>
+      <c r="KG12" s="11"/>
+      <c r="KH12" s="11"/>
+      <c r="KI12" s="11"/>
+      <c r="KJ12" s="11"/>
+      <c r="KK12" s="11"/>
+      <c r="KL12" s="11"/>
+      <c r="KM12" s="11"/>
+      <c r="KN12" s="11"/>
+      <c r="KO12" s="11"/>
+      <c r="KP12" s="11"/>
+      <c r="KQ12" s="11"/>
+      <c r="KR12" s="11"/>
+      <c r="KS12" s="11"/>
+      <c r="KT12" s="11"/>
+      <c r="KU12" s="11"/>
+      <c r="KV12" s="11"/>
+      <c r="KW12" s="11"/>
+      <c r="KX12" s="11"/>
+      <c r="KY12" s="11"/>
+      <c r="KZ12" s="11"/>
+      <c r="LA12" s="11"/>
+      <c r="LB12" s="11"/>
+      <c r="LC12" s="11"/>
+      <c r="LD12" s="11"/>
+      <c r="LE12" s="11"/>
+      <c r="LF12" s="11"/>
+      <c r="LG12" s="11"/>
+      <c r="LH12" s="11"/>
+      <c r="LI12" s="11"/>
+      <c r="LJ12" s="11"/>
+      <c r="LK12" s="11"/>
+      <c r="LL12" s="11"/>
+      <c r="LM12" s="11"/>
+      <c r="LN12" s="11"/>
+      <c r="LO12" s="11"/>
+      <c r="LP12" s="11"/>
+      <c r="LQ12" s="11"/>
+      <c r="LR12" s="11"/>
+      <c r="LS12" s="11"/>
+      <c r="LT12" s="11"/>
+      <c r="LU12" s="11"/>
+      <c r="LV12" s="11"/>
+      <c r="LW12" s="11"/>
+      <c r="LX12" s="11"/>
+      <c r="LY12" s="11"/>
+      <c r="LZ12" s="11"/>
+      <c r="MA12" s="11"/>
+      <c r="MB12" s="11"/>
+      <c r="MC12" s="11"/>
+      <c r="MD12" s="11"/>
+      <c r="ME12" s="11"/>
+      <c r="MF12" s="11"/>
+      <c r="MG12" s="11"/>
+      <c r="MH12" s="11"/>
+      <c r="MI12" s="11"/>
+      <c r="MJ12" s="11"/>
+      <c r="MK12" s="11"/>
+      <c r="ML12" s="11"/>
+      <c r="MM12" s="11"/>
+      <c r="MN12" s="11"/>
+      <c r="MO12" s="11"/>
+      <c r="MP12" s="11"/>
+      <c r="MQ12" s="11"/>
+      <c r="MR12" s="11"/>
+      <c r="MS12" s="11"/>
+      <c r="MT12" s="11"/>
+      <c r="MU12" s="11"/>
+      <c r="MV12" s="11"/>
+      <c r="MW12" s="11"/>
+      <c r="MX12" s="11"/>
+      <c r="MY12" s="11"/>
       <c r="MZ12" s="13"/>
       <c r="NA12" s="13"/>
       <c r="NB12" s="13"/>
@@ -15315,222 +13871,78 @@
       <c r="KE13" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="KF13" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KG13" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KH13" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KI13" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KJ13" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KK13" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KL13" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KM13" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KN13" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KO13" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KP13" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KQ13" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KR13" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KS13" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KT13" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KU13" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KV13" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KW13" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KX13" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KY13" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KZ13" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LA13" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LB13" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LC13" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LD13" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LE13" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LF13" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LG13" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LH13" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LI13" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LJ13" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LK13" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LL13" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LM13" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LN13" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LO13" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LP13" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LQ13" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LR13" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LS13" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LT13" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LU13" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LV13" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LW13" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LX13" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LY13" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LZ13" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MA13" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MB13" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MC13" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MD13" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="ME13" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MF13" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MG13" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MH13" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MI13" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MJ13" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MK13" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="ML13" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MM13" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MN13" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MO13" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MP13" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MQ13" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MR13" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MS13" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MT13" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MU13" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MV13" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MW13" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MX13" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MY13" s="11" t="n">
-        <v>0</v>
-      </c>
+      <c r="KF13" s="11"/>
+      <c r="KG13" s="11"/>
+      <c r="KH13" s="11"/>
+      <c r="KI13" s="11"/>
+      <c r="KJ13" s="11"/>
+      <c r="KK13" s="11"/>
+      <c r="KL13" s="11"/>
+      <c r="KM13" s="11"/>
+      <c r="KN13" s="11"/>
+      <c r="KO13" s="11"/>
+      <c r="KP13" s="11"/>
+      <c r="KQ13" s="11"/>
+      <c r="KR13" s="11"/>
+      <c r="KS13" s="11"/>
+      <c r="KT13" s="11"/>
+      <c r="KU13" s="11"/>
+      <c r="KV13" s="11"/>
+      <c r="KW13" s="11"/>
+      <c r="KX13" s="11"/>
+      <c r="KY13" s="11"/>
+      <c r="KZ13" s="11"/>
+      <c r="LA13" s="11"/>
+      <c r="LB13" s="11"/>
+      <c r="LC13" s="11"/>
+      <c r="LD13" s="11"/>
+      <c r="LE13" s="11"/>
+      <c r="LF13" s="11"/>
+      <c r="LG13" s="11"/>
+      <c r="LH13" s="11"/>
+      <c r="LI13" s="11"/>
+      <c r="LJ13" s="11"/>
+      <c r="LK13" s="11"/>
+      <c r="LL13" s="11"/>
+      <c r="LM13" s="11"/>
+      <c r="LN13" s="11"/>
+      <c r="LO13" s="11"/>
+      <c r="LP13" s="11"/>
+      <c r="LQ13" s="11"/>
+      <c r="LR13" s="11"/>
+      <c r="LS13" s="11"/>
+      <c r="LT13" s="11"/>
+      <c r="LU13" s="11"/>
+      <c r="LV13" s="11"/>
+      <c r="LW13" s="11"/>
+      <c r="LX13" s="11"/>
+      <c r="LY13" s="11"/>
+      <c r="LZ13" s="11"/>
+      <c r="MA13" s="11"/>
+      <c r="MB13" s="11"/>
+      <c r="MC13" s="11"/>
+      <c r="MD13" s="11"/>
+      <c r="ME13" s="11"/>
+      <c r="MF13" s="11"/>
+      <c r="MG13" s="11"/>
+      <c r="MH13" s="11"/>
+      <c r="MI13" s="11"/>
+      <c r="MJ13" s="11"/>
+      <c r="MK13" s="11"/>
+      <c r="ML13" s="11"/>
+      <c r="MM13" s="11"/>
+      <c r="MN13" s="11"/>
+      <c r="MO13" s="11"/>
+      <c r="MP13" s="11"/>
+      <c r="MQ13" s="11"/>
+      <c r="MR13" s="11"/>
+      <c r="MS13" s="11"/>
+      <c r="MT13" s="11"/>
+      <c r="MU13" s="11"/>
+      <c r="MV13" s="11"/>
+      <c r="MW13" s="11"/>
+      <c r="MX13" s="11"/>
+      <c r="MY13" s="11"/>
       <c r="MZ13" s="13"/>
       <c r="NA13" s="13"/>
       <c r="NB13" s="13"/>
@@ -16414,222 +14826,78 @@
       <c r="KE14" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="KF14" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KG14" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KH14" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KI14" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KJ14" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KK14" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KL14" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KM14" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KN14" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KO14" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KP14" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KQ14" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KR14" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KS14" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KT14" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KU14" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KV14" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KW14" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KX14" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KY14" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KZ14" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LA14" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LB14" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LC14" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LD14" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LE14" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LF14" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LG14" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LH14" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LI14" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LJ14" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LK14" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LL14" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LM14" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LN14" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LO14" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LP14" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LQ14" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LR14" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LS14" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LT14" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LU14" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LV14" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LW14" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LX14" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LY14" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LZ14" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MA14" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MB14" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MC14" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MD14" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="ME14" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MF14" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MG14" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MH14" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MI14" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MJ14" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MK14" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="ML14" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MM14" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MN14" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MO14" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MP14" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MQ14" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MR14" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MS14" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MT14" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MU14" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MV14" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MW14" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MX14" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MY14" s="11" t="n">
-        <v>0</v>
-      </c>
+      <c r="KF14" s="11"/>
+      <c r="KG14" s="11"/>
+      <c r="KH14" s="11"/>
+      <c r="KI14" s="11"/>
+      <c r="KJ14" s="11"/>
+      <c r="KK14" s="11"/>
+      <c r="KL14" s="11"/>
+      <c r="KM14" s="11"/>
+      <c r="KN14" s="11"/>
+      <c r="KO14" s="11"/>
+      <c r="KP14" s="11"/>
+      <c r="KQ14" s="11"/>
+      <c r="KR14" s="11"/>
+      <c r="KS14" s="11"/>
+      <c r="KT14" s="11"/>
+      <c r="KU14" s="11"/>
+      <c r="KV14" s="11"/>
+      <c r="KW14" s="11"/>
+      <c r="KX14" s="11"/>
+      <c r="KY14" s="11"/>
+      <c r="KZ14" s="11"/>
+      <c r="LA14" s="11"/>
+      <c r="LB14" s="11"/>
+      <c r="LC14" s="11"/>
+      <c r="LD14" s="11"/>
+      <c r="LE14" s="11"/>
+      <c r="LF14" s="11"/>
+      <c r="LG14" s="11"/>
+      <c r="LH14" s="11"/>
+      <c r="LI14" s="11"/>
+      <c r="LJ14" s="11"/>
+      <c r="LK14" s="11"/>
+      <c r="LL14" s="11"/>
+      <c r="LM14" s="11"/>
+      <c r="LN14" s="11"/>
+      <c r="LO14" s="11"/>
+      <c r="LP14" s="11"/>
+      <c r="LQ14" s="11"/>
+      <c r="LR14" s="11"/>
+      <c r="LS14" s="11"/>
+      <c r="LT14" s="11"/>
+      <c r="LU14" s="11"/>
+      <c r="LV14" s="11"/>
+      <c r="LW14" s="11"/>
+      <c r="LX14" s="11"/>
+      <c r="LY14" s="11"/>
+      <c r="LZ14" s="11"/>
+      <c r="MA14" s="11"/>
+      <c r="MB14" s="11"/>
+      <c r="MC14" s="11"/>
+      <c r="MD14" s="11"/>
+      <c r="ME14" s="11"/>
+      <c r="MF14" s="11"/>
+      <c r="MG14" s="11"/>
+      <c r="MH14" s="11"/>
+      <c r="MI14" s="11"/>
+      <c r="MJ14" s="11"/>
+      <c r="MK14" s="11"/>
+      <c r="ML14" s="11"/>
+      <c r="MM14" s="11"/>
+      <c r="MN14" s="11"/>
+      <c r="MO14" s="11"/>
+      <c r="MP14" s="11"/>
+      <c r="MQ14" s="11"/>
+      <c r="MR14" s="11"/>
+      <c r="MS14" s="11"/>
+      <c r="MT14" s="11"/>
+      <c r="MU14" s="11"/>
+      <c r="MV14" s="11"/>
+      <c r="MW14" s="11"/>
+      <c r="MX14" s="11"/>
+      <c r="MY14" s="11"/>
       <c r="MZ14" s="13"/>
       <c r="NA14" s="13"/>
       <c r="NB14" s="13"/>

</xml_diff>